<commit_message>
chore(UX): Update jdt et deux ajout des 2 personas
</commit_message>
<xml_diff>
--- a/UX/jdt/T_ShootMeUp-matolaya.xlsx
+++ b/UX/jdt/T_ShootMeUp-matolaya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg24muu\Documents\GitHub\P_ShootMeUp\UX\jdt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D159630-310C-42FD-AE08-404FC3892764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A77725A-87DA-4D19-AF8A-015561F5FE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Auteur:</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t xml:space="preserve">Je n'ai pas eu le temps de le terminer </t>
+  </si>
+  <si>
+    <t>Finir le second persona</t>
+  </si>
+  <si>
+    <t>Instructions et exemples données par le prof.</t>
+  </si>
+  <si>
+    <t>Commencer la création des Wireframes.</t>
+  </si>
+  <si>
+    <t>J'ai commencé la maquette main menu</t>
   </si>
 </sst>
 </file>
@@ -1085,16 +1097,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1937,16 +1949,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.8666666666666667</c:v>
+                  <c:v>0.69696969696969702</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>9.0909090909090912E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13333333333333333</c:v>
+                  <c:v>0.21212121212121213</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4130,9 +4142,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4187,7 +4199,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>1 heures 15 minutes</v>
+        <v>2 heures 45 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4206,11 +4218,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>75</v>
+        <v>165</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>75</v>
+        <v>165</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4325,15 +4337,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="73" t="str">
+      <c r="A10" s="73">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="36"/>
+        <v>36</v>
+      </c>
+      <c r="B10" s="36">
+        <v>45541</v>
+      </c>
       <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="28"/>
+      <c r="D10" s="38">
+        <v>50</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="G10" s="45"/>
       <c r="M10" t="s">
         <v>3</v>
@@ -4346,15 +4366,23 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="str">
+      <c r="A11" s="74">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="40"/>
+        <v>36</v>
+      </c>
+      <c r="B11" s="40">
+        <v>45541</v>
+      </c>
       <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="28"/>
+      <c r="D11" s="42">
+        <v>25</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>36</v>
+      </c>
       <c r="G11" s="46"/>
       <c r="M11" t="s">
         <v>4</v>
@@ -4367,16 +4395,26 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="73" t="str">
+      <c r="A12" s="73">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="36"/>
+        <v>36</v>
+      </c>
+      <c r="B12" s="36">
+        <v>45541</v>
+      </c>
       <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="45"/>
+      <c r="D12" s="38">
+        <v>15</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="45" t="s">
+        <v>38</v>
+      </c>
       <c r="N12">
         <v>5</v>
       </c>
@@ -10713,7 +10751,7 @@
   <dimension ref="A2:N12"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -10794,11 +10832,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10806,11 +10844,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>1 h 05 min</v>
+        <v>1 h 55 min</v>
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.8666666666666667</v>
+        <v>0.69696969696969702</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10831,11 +10869,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10843,11 +10881,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 00 min</v>
+        <v>0 h 15 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10905,11 +10943,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10917,11 +10955,11 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>0 h 10 min</v>
+        <v>0 h 35 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.13333333333333333</v>
+        <v>0.21212121212121213</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10942,22 +10980,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>75</v>
+        <v>165</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>75</v>
+        <v>165</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 15 min</v>
+        <v>2 h 45 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>1.4204545454545454E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11001,6 +11039,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="34298955776df91f451dfdd912b0d80d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed9741631eefaa61c396a6d47d02de0f" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11195,27 +11253,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EE95A31-3997-42E6-AE6E-094AD61D4048}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11232,25 +11291,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(assets): amelioration de l'asset
</commit_message>
<xml_diff>
--- a/UX/jdt/T_ShootMeUp-matolaya.xlsx
+++ b/UX/jdt/T_ShootMeUp-matolaya.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg24muu\Documents\GitHub\P_ShootMeUp\UX\jdt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79391A6-3AC7-465B-A0AF-DCC0C96CBAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E669349-D884-4789-99F3-BC944FFD6D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="29925" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -11102,6 +11102,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="34298955776df91f451dfdd912b0d80d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed9741631eefaa61c396a6d47d02de0f" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11296,27 +11316,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EE95A31-3997-42E6-AE6E-094AD61D4048}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11333,25 +11354,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>